<commit_message>
ci sono arrivato in fondo
</commit_message>
<xml_diff>
--- a/dati/liste.xlsx
+++ b/dati/liste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Repos\elezioni-EMR\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB27ABD-1C33-41DD-8FF3-7866E421E898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C055BC-97B1-4C81-AEB7-5D9423525854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>SINISTRA</t>
   </si>
@@ -93,6 +93,39 @@
   </si>
   <si>
     <t>astensione</t>
+  </si>
+  <si>
+    <t>COLORE</t>
+  </si>
+  <si>
+    <t>#FF0000</t>
+  </si>
+  <si>
+    <t>#00FF00</t>
+  </si>
+  <si>
+    <t>#FFA500</t>
+  </si>
+  <si>
+    <t>#FFFF00</t>
+  </si>
+  <si>
+    <t>#ff268f</t>
+  </si>
+  <si>
+    <t>#26ffba</t>
+  </si>
+  <si>
+    <t>#2945e3</t>
+  </si>
+  <si>
+    <t>#00d5ff</t>
+  </si>
+  <si>
+    <t>#001f9c</t>
+  </si>
+  <si>
+    <t>#3086db</t>
   </si>
 </sst>
 </file>
@@ -432,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +478,7 @@
     <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -455,8 +488,11 @@
       <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -466,8 +502,11 @@
       <c r="C2" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -477,8 +516,11 @@
       <c r="C3" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -488,8 +530,11 @@
       <c r="C4" s="2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -499,8 +544,11 @@
       <c r="C5" s="2">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -510,8 +558,11 @@
       <c r="C6" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -521,8 +572,11 @@
       <c r="C7" s="2">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -532,8 +586,11 @@
       <c r="C8" s="2">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -543,8 +600,11 @@
       <c r="C9" s="2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -554,8 +614,11 @@
       <c r="C10" s="2">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -565,8 +628,11 @@
       <c r="C11" s="2">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -577,7 +643,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
inizio conversione a data.table
</commit_message>
<xml_diff>
--- a/dati/liste.xlsx
+++ b/dati/liste.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Repos\elezioni-EMR\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE17698-6041-46B9-A416-6D9790749080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4492F2B7-E217-4AFB-A2D2-64BE8B2AB322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="europee" sheetId="2" r:id="rId2"/>
+    <sheet name="liste_europee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="42">
   <si>
     <t>SINISTRA</t>
   </si>
@@ -506,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,4 +1888,126 @@
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7545EAE8-68D8-420C-A1A7-4F763ECC112D}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>